<commit_message>
Matching GUI displays, but no methods attached
</commit_message>
<xml_diff>
--- a/Structure and plan info/Report_tables.xlsx
+++ b/Structure and plan info/Report_tables.xlsx
@@ -1,37 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://queensuca-my.sharepoint.com/personal/gs13_queensu_ca/Documents/Python/Projects/EclipseRelated/PlanEvaluation/Structure and plan info/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="39" documentId="11_D0EC9C8AFE3384CF55C5FE9AC2406CE4AB4B1569" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{12B5D73E-A692-4CBF-9790-58BEF1B268A5}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="16335" windowHeight="10830"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15060" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EvaluationSheet 48Gy4F 60Gy5F" sheetId="5" r:id="rId1"/>
-    <sheet name="SABR 48 in 4" sheetId="4" r:id="rId2"/>
-    <sheet name="EvaluationSheet 60Gy 8F" sheetId="6" r:id="rId3"/>
-    <sheet name="SABR 60 in 8" sheetId="3" r:id="rId4"/>
-    <sheet name="EvaluationSheet 54Gy 3F" sheetId="7" r:id="rId5"/>
-    <sheet name="SABR 54 in 3" sheetId="1" r:id="rId6"/>
-    <sheet name="CELL format codes" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
+    <sheet name="SABR 48 in 4" sheetId="4" r:id="rId3"/>
+    <sheet name="EvaluationSheet 60Gy 8F" sheetId="6" r:id="rId4"/>
+    <sheet name="SABR 60 in 8" sheetId="3" r:id="rId5"/>
+    <sheet name="EvaluationSheet 54Gy 3F" sheetId="7" r:id="rId6"/>
+    <sheet name="SABR 54 in 3" sheetId="1" r:id="rId7"/>
+    <sheet name="CELL format codes" sheetId="8" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
-    <definedName name="B" localSheetId="6">#REF!</definedName>
+    <definedName name="B" localSheetId="7">#REF!</definedName>
     <definedName name="B">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'EvaluationSheet 48Gy4F 60Gy5F'!$B$2:$L$62</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'EvaluationSheet 54Gy 3F'!$B$2:$L$52</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'EvaluationSheet 60Gy 8F'!$B$2:$L$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'EvaluationSheet 54Gy 3F'!$B$2:$L$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'EvaluationSheet 60Gy 8F'!$B$2:$L$53</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3286" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3344" uniqueCount="505">
   <si>
     <t>Aliases</t>
   </si>
@@ -2722,11 +2736,38 @@
   <si>
     <t>Format</t>
   </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Ipsilateral</t>
+  </si>
+  <si>
+    <t>Proximal</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Direct Entry</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -4241,6 +4282,16 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4255,91 +4306,201 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Heading 1" xfId="4" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="5"/>
-    <cellStyle name="Percent 2" xfId="2"/>
-    <cellStyle name="Percent 3" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Percent 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Percent 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="36">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thick">
+          <color theme="4"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -4619,17 +4780,77 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
-        </top>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -4665,191 +4886,14 @@
       </fill>
       <protection locked="1" hidden="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thick">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -4982,52 +5026,15 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="SABR 60 in 8"/>
-      <sheetName val="SABR 60 in 8 Log"/>
-      <sheetName val="EvaluationSheet 60Gy 8F"/>
-      <sheetName val="Report Reference 60 in 8.txt"/>
-      <sheetName val="SABR 48 in 4"/>
-      <sheetName val="SABR 48 in 4 Log"/>
-      <sheetName val="EvaluationSheet 48Gy4F 60Gy5F"/>
-      <sheetName val="Report Reference 48 in 4.txt"/>
-      <sheetName val="54Gy 3F"/>
-      <sheetName val="54Gy 3F Log"/>
-      <sheetName val="EvaluationSheet 54Gy 3F"/>
-      <sheetName val="CELL format codes"/>
-      <sheetName val="xml cell values"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Report_48in4" displayName="Report_48in4" ref="O3:R57" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Report_48in4" displayName="Report_48in4" ref="O3:R57" totalsRowShown="0">
   <tableColumns count="4">
-    <tableColumn id="1" name="Label" dataDxfId="16" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" name="Cell Address" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" name="Value" dataDxfId="15" dataCellStyle="Normal 2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label" dataDxfId="35" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Cell Address" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Value" dataDxfId="34" dataCellStyle="Normal 2">
       <calculatedColumnFormula>INDIRECT(P4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Format" dataCellStyle="Normal 2">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Format" dataCellStyle="Normal 2">
       <calculatedColumnFormula>VLOOKUP(CELL("format",INDIRECT(P4)),CellFormatCodes[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5036,29 +5043,29 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="ReportDef_48in4" displayName="ReportDef_48in4" ref="T3:AD57" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="13" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ReportDef_48in4" displayName="ReportDef_48in4" ref="T3:AD57" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30">
   <tableColumns count="11">
-    <tableColumn id="1" name="Item Name" dataDxfId="12"/>
-    <tableColumn id="2" name="Item Label" dataDxfId="11"/>
-    <tableColumn id="3" name="CellAddress" dataDxfId="10"/>
-    <tableColumn id="4" name="Unit" dataDxfId="9"/>
-    <tableColumn id="5" name="CellFormat" dataDxfId="8"/>
-    <tableColumn id="6" name="Item Category" dataDxfId="7"/>
-    <tableColumn id="7" name="reference_type" dataDxfId="6"/>
-    <tableColumn id="8" name="reference_name" dataDxfId="5"/>
-    <tableColumn id="9" name="reference_laterality" dataDxfId="4"/>
-    <tableColumn id="10" name="Aliases" dataDxfId="3"/>
-    <tableColumn id="11" name="constructor" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Item Name" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Item Label" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="CellAddress" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Unit" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="CellFormat" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Item Category" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="reference_type" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="reference_name" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="reference_laterality" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Aliases" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="constructor" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="CellFormatCodes" displayName="CellFormatCodes" ref="A2:B27" totalsRowShown="0" tableBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="CellFormatCodes" displayName="CellFormatCodes" ref="A2:B27" totalsRowShown="0" tableBorderDxfId="18">
   <tableColumns count="2">
-    <tableColumn id="1" name="Code"/>
-    <tableColumn id="2" name="Format Text" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Code"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Format Text" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5107,7 +5114,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5140,9 +5147,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5175,6 +5199,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5350,14 +5391,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AD69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5385,7 +5426,7 @@
     <col min="21" max="21" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13.85546875" customWidth="1"/>
     <col min="23" max="23" width="6.7109375" customWidth="1"/>
-    <col min="24" max="24" width="13.140625" style="279" customWidth="1"/>
+    <col min="24" max="24" width="13.140625" style="271" customWidth="1"/>
     <col min="25" max="25" width="15.85546875" customWidth="1"/>
     <col min="26" max="26" width="16.7109375" customWidth="1"/>
     <col min="27" max="27" width="32.5703125" bestFit="1" customWidth="1"/>
@@ -5429,12 +5470,12 @@
       <c r="K2" s="16"/>
       <c r="L2" s="18"/>
       <c r="M2" s="10"/>
-      <c r="O2" s="278" t="s">
+      <c r="O2" s="281" t="s">
         <v>442</v>
       </c>
-      <c r="P2" s="278"/>
-      <c r="Q2" s="278"/>
-      <c r="R2" s="278"/>
+      <c r="P2" s="281"/>
+      <c r="Q2" s="281"/>
+      <c r="R2" s="281"/>
     </row>
     <row r="3" spans="2:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="19"/>
@@ -5463,37 +5504,37 @@
       <c r="R3" s="11" t="s">
         <v>495</v>
       </c>
-      <c r="T3" s="281" t="s">
+      <c r="T3" s="273" t="s">
         <v>5</v>
       </c>
-      <c r="U3" s="281" t="s">
+      <c r="U3" s="273" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="281" t="s">
+      <c r="V3" s="273" t="s">
         <v>1</v>
       </c>
-      <c r="W3" s="281" t="s">
+      <c r="W3" s="273" t="s">
         <v>11</v>
       </c>
-      <c r="X3" s="282" t="s">
+      <c r="X3" s="274" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="281" t="s">
+      <c r="Y3" s="273" t="s">
         <v>3</v>
       </c>
-      <c r="Z3" s="281" t="s">
+      <c r="Z3" s="273" t="s">
         <v>16</v>
       </c>
-      <c r="AA3" s="281" t="s">
+      <c r="AA3" s="273" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="281" t="s">
+      <c r="AB3" s="273" t="s">
         <v>14</v>
       </c>
-      <c r="AC3" s="281" t="s">
+      <c r="AC3" s="273" t="s">
         <v>0</v>
       </c>
-      <c r="AD3" s="281" t="s">
+      <c r="AD3" s="273" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5542,7 +5583,7 @@
         <v>18</v>
       </c>
       <c r="W4" s="3"/>
-      <c r="X4" s="280" t="s">
+      <c r="X4" s="272" t="s">
         <v>58</v>
       </c>
       <c r="Y4" s="3" t="s">
@@ -5603,7 +5644,7 @@
         <v>19</v>
       </c>
       <c r="W5" s="3"/>
-      <c r="X5" s="280" t="s">
+      <c r="X5" s="272" t="s">
         <v>59</v>
       </c>
       <c r="Y5" s="3" t="s">
@@ -5660,7 +5701,7 @@
         <v>20</v>
       </c>
       <c r="W6" s="3"/>
-      <c r="X6" s="280" t="s">
+      <c r="X6" s="272" t="s">
         <v>59</v>
       </c>
       <c r="Y6" s="3" t="s">
@@ -5717,7 +5758,7 @@
         <v>21</v>
       </c>
       <c r="W7" s="3"/>
-      <c r="X7" s="280" t="s">
+      <c r="X7" s="272" t="s">
         <v>59</v>
       </c>
       <c r="Y7" s="3" t="s">
@@ -5776,7 +5817,7 @@
       <c r="W8" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X8" s="280" t="s">
+      <c r="X8" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y8" s="3" t="s">
@@ -5837,7 +5878,7 @@
       <c r="W9" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X9" s="280" t="s">
+      <c r="X9" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y9" s="3" t="s">
@@ -5898,7 +5939,7 @@
       <c r="W10" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X10" s="280" t="s">
+      <c r="X10" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y10" s="3" t="s">
@@ -5967,7 +6008,7 @@
       <c r="W11" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X11" s="280" t="s">
+      <c r="X11" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y11" s="3" t="s">
@@ -6038,7 +6079,7 @@
       <c r="W12" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X12" s="280" t="s">
+      <c r="X12" s="272" t="s">
         <v>58</v>
       </c>
       <c r="Y12" s="3" t="s">
@@ -6097,7 +6138,7 @@
         <v>27</v>
       </c>
       <c r="W13" s="3"/>
-      <c r="X13" s="280" t="s">
+      <c r="X13" s="272" t="s">
         <v>61</v>
       </c>
       <c r="Y13" s="3" t="s">
@@ -6165,7 +6206,7 @@
       <c r="W14" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="X14" s="280" t="s">
+      <c r="X14" s="272" t="s">
         <v>62</v>
       </c>
       <c r="Y14" s="3" t="s">
@@ -6235,7 +6276,7 @@
       <c r="W15" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="X15" s="280" t="s">
+      <c r="X15" s="272" t="s">
         <v>62</v>
       </c>
       <c r="Y15" s="3" t="s">
@@ -6296,7 +6337,7 @@
       <c r="W16" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="X16" s="280" t="s">
+      <c r="X16" s="272" t="s">
         <v>62</v>
       </c>
       <c r="Y16" s="3" t="s">
@@ -6364,7 +6405,7 @@
       <c r="W17" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="X17" s="280" t="s">
+      <c r="X17" s="272" t="s">
         <v>62</v>
       </c>
       <c r="Y17" s="3" t="s">
@@ -6434,7 +6475,7 @@
       <c r="W18" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X18" s="280" t="s">
+      <c r="X18" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y18" s="3" t="s">
@@ -6506,7 +6547,7 @@
       <c r="W19" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X19" s="280" t="s">
+      <c r="X19" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y19" s="3" t="s">
@@ -6567,7 +6608,7 @@
       <c r="W20" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="X20" s="280" t="s">
+      <c r="X20" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y20" s="3" t="s">
@@ -6644,7 +6685,7 @@
       <c r="W21" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X21" s="280" t="s">
+      <c r="X21" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y21" s="3" t="s">
@@ -6723,7 +6764,7 @@
       <c r="W22" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X22" s="280" t="s">
+      <c r="X22" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y22" s="3" t="s">
@@ -6786,7 +6827,7 @@
       <c r="W23" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X23" s="280" t="s">
+      <c r="X23" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y23" s="3" t="s">
@@ -6863,7 +6904,7 @@
       <c r="W24" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="X24" s="280" t="s">
+      <c r="X24" s="272" t="s">
         <v>62</v>
       </c>
       <c r="Y24" s="3" t="s">
@@ -6945,7 +6986,7 @@
       <c r="W25" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X25" s="280" t="s">
+      <c r="X25" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y25" s="3" t="s">
@@ -7014,7 +7055,7 @@
       <c r="W26" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X26" s="280" t="s">
+      <c r="X26" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y26" s="3" t="s">
@@ -7081,7 +7122,7 @@
       <c r="W27" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X27" s="280" t="s">
+      <c r="X27" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y27" s="3" t="s">
@@ -7121,7 +7162,7 @@
         <v>Aorta  (max point dose)</v>
       </c>
       <c r="P28" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G35),"$","")</f>
+        <f t="shared" ref="P28:P45" ca="1" si="1">SUBSTITUTE(CELL("address",G35),"$","")</f>
         <v>G35</v>
       </c>
       <c r="Q28" s="96" t="str">
@@ -7144,7 +7185,7 @@
       <c r="W28" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X28" s="280" t="s">
+      <c r="X28" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y28" s="3" t="s">
@@ -7186,7 +7227,7 @@
         <v>Aorta  V40Gy=</v>
       </c>
       <c r="P29" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G36),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G36</v>
       </c>
       <c r="Q29" s="96" t="str">
@@ -7209,7 +7250,7 @@
       <c r="W29" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X29" s="280" t="s">
+      <c r="X29" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y29" s="3" t="s">
@@ -7251,7 +7292,7 @@
         <v>Artery-Pulmonary (max point dose)</v>
       </c>
       <c r="P30" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G37),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G37</v>
       </c>
       <c r="Q30" s="96" t="str">
@@ -7274,7 +7315,7 @@
       <c r="W30" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X30" s="280" t="s">
+      <c r="X30" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y30" s="3" t="s">
@@ -7298,10 +7339,10 @@
         <v>340</v>
       </c>
       <c r="D31" s="27"/>
-      <c r="E31" s="269" t="s">
+      <c r="E31" s="275" t="s">
         <v>341</v>
       </c>
-      <c r="F31" s="270"/>
+      <c r="F31" s="276"/>
       <c r="G31" s="76" t="s">
         <v>310</v>
       </c>
@@ -7325,7 +7366,7 @@
         <v>Artery-Pulmonary V40Gy=</v>
       </c>
       <c r="P31" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G38),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G38</v>
       </c>
       <c r="Q31" s="96" t="str">
@@ -7348,7 +7389,7 @@
       <c r="W31" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X31" s="280" t="s">
+      <c r="X31" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y31" s="3" t="s">
@@ -7372,10 +7413,10 @@
         <v>88</v>
       </c>
       <c r="D32" s="27"/>
-      <c r="E32" s="269" t="s">
+      <c r="E32" s="275" t="s">
         <v>344</v>
       </c>
-      <c r="F32" s="270"/>
+      <c r="F32" s="276"/>
       <c r="G32" s="92" t="s">
         <v>310</v>
       </c>
@@ -7397,7 +7438,7 @@
         <v>Spinal Canal (max point dose)</v>
       </c>
       <c r="P32" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G39),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G39</v>
       </c>
       <c r="Q32" s="96" t="str">
@@ -7420,7 +7461,7 @@
       <c r="W32" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X32" s="280" t="s">
+      <c r="X32" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y32" s="3" t="s">
@@ -7444,10 +7485,10 @@
         <v>89</v>
       </c>
       <c r="D33" s="27"/>
-      <c r="E33" s="271" t="s">
+      <c r="E33" s="277" t="s">
         <v>346</v>
       </c>
-      <c r="F33" s="272"/>
+      <c r="F33" s="278"/>
       <c r="G33" s="135" t="s">
         <v>310</v>
       </c>
@@ -7469,7 +7510,7 @@
         <v>Spinal Canal V20.8Gy=</v>
       </c>
       <c r="P33" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G40),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G40</v>
       </c>
       <c r="Q33" s="96" t="str">
@@ -7492,7 +7533,7 @@
       <c r="W33" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X33" s="280" t="s">
+      <c r="X33" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y33" s="3" t="s">
@@ -7532,7 +7573,7 @@
         <v>Spinal Canal V13.6Gy=</v>
       </c>
       <c r="P34" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G41),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G41</v>
       </c>
       <c r="Q34" s="96" t="str">
@@ -7555,7 +7596,7 @@
       <c r="W34" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X34" s="280" t="s">
+      <c r="X34" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y34" s="3" t="s">
@@ -7606,7 +7647,7 @@
         <v>Spinal Canal-PRV 5mm (max point dose)</v>
       </c>
       <c r="P35" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G42),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G42</v>
       </c>
       <c r="Q35" s="96" t="str">
@@ -7629,7 +7670,7 @@
       <c r="W35" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X35" s="280" t="s">
+      <c r="X35" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y35" s="3" t="s">
@@ -7681,7 +7722,7 @@
         <v>Ipsilat. Brach. Plex. (max point dose)</v>
       </c>
       <c r="P36" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G43),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G43</v>
       </c>
       <c r="Q36" s="96" t="str">
@@ -7704,7 +7745,7 @@
       <c r="W36" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X36" s="280" t="s">
+      <c r="X36" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y36" s="3" t="s">
@@ -7755,7 +7796,7 @@
         <v>Ipsilat. Brach. Plex. V23.6Gy=</v>
       </c>
       <c r="P37" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G44),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G44</v>
       </c>
       <c r="Q37" s="96" t="str">
@@ -7778,7 +7819,7 @@
       <c r="W37" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X37" s="280" t="s">
+      <c r="X37" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y37" s="3" t="s">
@@ -7828,7 +7869,7 @@
         <v>Skin V30Gy=</v>
       </c>
       <c r="P38" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G45),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G45</v>
       </c>
       <c r="Q38" s="96" t="str">
@@ -7851,7 +7892,7 @@
       <c r="W38" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X38" s="280" t="s">
+      <c r="X38" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y38" s="3" t="s">
@@ -7902,7 +7943,7 @@
         <v>Heart (max point dose)</v>
       </c>
       <c r="P39" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G46),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G46</v>
       </c>
       <c r="Q39" s="96" t="str">
@@ -7925,7 +7966,7 @@
       <c r="W39" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X39" s="280" t="s">
+      <c r="X39" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y39" s="3" t="s">
@@ -7946,10 +7987,10 @@
     <row r="40" spans="2:30" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B40" s="24"/>
       <c r="C40" s="24"/>
-      <c r="D40" s="273" t="s">
+      <c r="D40" s="279" t="s">
         <v>355</v>
       </c>
-      <c r="E40" s="274"/>
+      <c r="E40" s="280"/>
       <c r="F40" s="146" t="s">
         <v>356</v>
       </c>
@@ -7975,7 +8016,7 @@
         <v>Heart V28Gy=</v>
       </c>
       <c r="P40" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G47),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G47</v>
       </c>
       <c r="Q40" s="96" t="str">
@@ -7998,7 +8039,7 @@
       <c r="W40" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X40" s="280" t="s">
+      <c r="X40" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y40" s="3" t="s">
@@ -8048,7 +8089,7 @@
         <v>Esophagus (max point dose)</v>
       </c>
       <c r="P41" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G48),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G48</v>
       </c>
       <c r="Q41" s="96" t="str">
@@ -8071,7 +8112,7 @@
       <c r="W41" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X41" s="280" t="s">
+      <c r="X41" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y41" s="3" t="s">
@@ -8118,7 +8159,7 @@
         <v>Esophagus V18.8Gy=</v>
       </c>
       <c r="P42" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G49),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G49</v>
       </c>
       <c r="Q42" s="96" t="str">
@@ -8141,7 +8182,7 @@
       <c r="W42" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X42" s="280" t="s">
+      <c r="X42" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y42" s="3" t="s">
@@ -8190,7 +8231,7 @@
         <v>*Chestwall (rib) (max point dose)</v>
       </c>
       <c r="P43" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G50),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G50</v>
       </c>
       <c r="Q43" s="96" t="str">
@@ -8213,7 +8254,7 @@
       <c r="W43" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X43" s="280" t="s">
+      <c r="X43" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y43" s="3" t="s">
@@ -8265,7 +8306,7 @@
         <v>*Chestwall (rib) V40Gy=</v>
       </c>
       <c r="P44" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G51),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G51</v>
       </c>
       <c r="Q44" s="96" t="str">
@@ -8288,7 +8329,7 @@
       <c r="W44" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X44" s="280" t="s">
+      <c r="X44" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y44" s="3" t="s">
@@ -8341,7 +8382,7 @@
         <v>*Chestwall (rib) V30Gy=</v>
       </c>
       <c r="P45" s="11" t="str">
-        <f ca="1">SUBSTITUTE(CELL("address",G52),"$","")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>G52</v>
       </c>
       <c r="Q45" s="96" t="str">
@@ -8364,7 +8405,7 @@
       <c r="W45" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X45" s="280" t="s">
+      <c r="X45" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y45" s="3" t="s">
@@ -8436,7 +8477,7 @@
       <c r="W46" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X46" s="280" t="s">
+      <c r="X46" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y46" s="3" t="s">
@@ -8511,7 +8552,7 @@
       <c r="W47" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X47" s="280" t="s">
+      <c r="X47" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y47" s="3" t="s">
@@ -8583,7 +8624,7 @@
       <c r="W48" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X48" s="280" t="s">
+      <c r="X48" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y48" s="3" t="s">
@@ -8654,7 +8695,7 @@
       <c r="W49" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="X49" s="280" t="s">
+      <c r="X49" s="272" t="s">
         <v>64</v>
       </c>
       <c r="Y49" s="3" t="s">
@@ -8726,7 +8767,7 @@
       <c r="W50" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="X50" s="280" t="s">
+      <c r="X50" s="272" t="s">
         <v>60</v>
       </c>
       <c r="Y50" s="3" t="s">
@@ -8797,7 +8838,7 @@
         <v>55</v>
       </c>
       <c r="W51" s="3"/>
-      <c r="X51" s="280" t="s">
+      <c r="X51" s="272" t="s">
         <v>62</v>
       </c>
       <c r="Y51" s="3" t="s">
@@ -8870,7 +8911,7 @@
         <v>56</v>
       </c>
       <c r="W52" s="3"/>
-      <c r="X52" s="280" t="s">
+      <c r="X52" s="272" t="s">
         <v>62</v>
       </c>
       <c r="Y52" s="3" t="s">
@@ -8948,7 +8989,7 @@
         <v>57</v>
       </c>
       <c r="W53" s="3"/>
-      <c r="X53" s="280" t="s">
+      <c r="X53" s="272" t="s">
         <v>62</v>
       </c>
       <c r="Y53" s="3" t="s">
@@ -9014,7 +9055,7 @@
         <v>491</v>
       </c>
       <c r="W54" s="3"/>
-      <c r="X54" s="280"/>
+      <c r="X54" s="272"/>
       <c r="Y54" s="3" t="s">
         <v>65</v>
       </c>
@@ -9088,7 +9129,7 @@
         <v>492</v>
       </c>
       <c r="W55" s="3"/>
-      <c r="X55" s="280"/>
+      <c r="X55" s="272"/>
       <c r="Y55" s="3" t="s">
         <v>65</v>
       </c>
@@ -9154,7 +9195,7 @@
         <v>493</v>
       </c>
       <c r="W56" s="3"/>
-      <c r="X56" s="280"/>
+      <c r="X56" s="272"/>
       <c r="Y56" s="3" t="s">
         <v>65</v>
       </c>
@@ -9377,31 +9418,31 @@
     <mergeCell ref="O2:R2"/>
   </mergeCells>
   <conditionalFormatting sqref="L35:L57">
-    <cfRule type="containsText" dxfId="33" priority="7" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="16" priority="7" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",L35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14:L20 L22:L33">
-    <cfRule type="containsText" dxfId="32" priority="4" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="15" priority="4" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",L14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="5" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="14" priority="5" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",L14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="6" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="13" priority="6" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",L14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="containsText" dxfId="29" priority="2" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="12" priority="2" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",L21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="3" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="11" priority="3" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",L21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="containsText" dxfId="27" priority="1" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="10" priority="1" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",L21)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9416,14 +9457,514 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D454F34-3465-470E-B7EA-BACA68E097AA}">
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D1">
+        <f>MAX(B2:B39)</f>
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B39" si="0">LEN(A2)</f>
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:H4" si="1">LEN(G2)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>199</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>497</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H16" si="2">LEN(G9)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>498</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>172</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>499</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>500</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>173</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>501</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>172</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H19" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>502</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20:H23" si="3">LEN(G20)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G21" t="s">
+        <v>503</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
+        <v>504</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
+        <v>499</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="3"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B39">
+    <sortCondition descending="1" ref="B2:B39"/>
+    <sortCondition ref="A2:A39"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12005,14 +12546,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R60"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
@@ -12988,10 +13529,10 @@
         <v>389</v>
       </c>
       <c r="D31" s="20"/>
-      <c r="E31" s="271" t="s">
+      <c r="E31" s="277" t="s">
         <v>341</v>
       </c>
-      <c r="F31" s="272"/>
+      <c r="F31" s="278"/>
       <c r="G31" s="82" t="s">
         <v>310</v>
       </c>
@@ -13857,42 +14398,42 @@
     <mergeCell ref="E31:F31"/>
   </mergeCells>
   <conditionalFormatting sqref="L33:L48">
-    <cfRule type="containsText" dxfId="26" priority="10" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="9" priority="10" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",L33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20:L30">
-    <cfRule type="containsText" dxfId="25" priority="8" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="8" priority="8" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",L20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="9" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="7" priority="9" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",L20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20:L25">
-    <cfRule type="containsText" dxfId="23" priority="7" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="6" priority="7" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",L20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L31">
-    <cfRule type="containsText" dxfId="22" priority="1" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="5" priority="1" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",L31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="2" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="4" priority="2" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",L31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="6" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="3" priority="6" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",L31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14:L19">
-    <cfRule type="containsText" dxfId="19" priority="3" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="2" priority="3" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",L14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="4" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="1" priority="4" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",L14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="5" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="0" priority="5" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",L14)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13902,14 +14443,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -16319,8 +16862,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -18092,14 +18635,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -20359,8 +20904,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20369,222 +20914,222 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="276" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" style="276" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="276"/>
+    <col min="1" max="1" width="7.7109375" style="269" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="269" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="269"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="275" t="s">
+      <c r="A1" s="282" t="s">
         <v>446</v>
       </c>
-      <c r="B1" s="275"/>
+      <c r="B1" s="282"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="276" t="s">
+      <c r="A2" s="269" t="s">
         <v>447</v>
       </c>
-      <c r="B2" s="276" t="s">
+      <c r="B2" s="269" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="276" t="s">
+      <c r="A3" s="269" t="s">
         <v>449</v>
       </c>
-      <c r="B3" s="277" t="s">
+      <c r="B3" s="270" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="276" t="s">
+      <c r="A4" s="269" t="s">
         <v>450</v>
       </c>
-      <c r="B4" s="277">
+      <c r="B4" s="270">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="276" t="s">
+      <c r="A5" s="269" t="s">
         <v>451</v>
       </c>
-      <c r="B5" s="277" t="s">
+      <c r="B5" s="270" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="276" t="s">
+      <c r="A6" s="269" t="s">
         <v>452</v>
       </c>
-      <c r="B6" s="277" t="s">
+      <c r="B6" s="270" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="276" t="s">
+      <c r="A7" s="269" t="s">
         <v>453</v>
       </c>
-      <c r="B7" s="277" t="s">
+      <c r="B7" s="270" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="276" t="s">
+      <c r="A8" s="269" t="s">
         <v>455</v>
       </c>
-      <c r="B8" s="277" t="s">
+      <c r="B8" s="270" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="276" t="s">
+      <c r="A9" s="269" t="s">
         <v>457</v>
       </c>
-      <c r="B9" s="277" t="s">
+      <c r="B9" s="270" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="276" t="s">
+      <c r="A10" s="269" t="s">
         <v>459</v>
       </c>
-      <c r="B10" s="277" t="s">
+      <c r="B10" s="270" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="276" t="s">
+      <c r="A11" s="269" t="s">
         <v>461</v>
       </c>
-      <c r="B11" s="277" t="s">
+      <c r="B11" s="270" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="276" t="s">
+      <c r="A12" s="269" t="s">
         <v>463</v>
       </c>
-      <c r="B12" s="277" t="s">
+      <c r="B12" s="270" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="276" t="s">
+      <c r="A13" s="269" t="s">
         <v>465</v>
       </c>
-      <c r="B13" s="277" t="s">
+      <c r="B13" s="270" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="276" t="s">
+      <c r="A14" s="269" t="s">
         <v>467</v>
       </c>
-      <c r="B14" s="277" t="s">
+      <c r="B14" s="270" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="276" t="s">
+      <c r="A15" s="269" t="s">
         <v>469</v>
       </c>
-      <c r="B15" s="277" t="s">
+      <c r="B15" s="270" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="276" t="s">
+      <c r="A16" s="269" t="s">
         <v>470</v>
       </c>
-      <c r="B16" s="277" t="s">
+      <c r="B16" s="270" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="276" t="s">
+      <c r="A17" s="269" t="s">
         <v>471</v>
       </c>
-      <c r="B17" s="277" t="s">
+      <c r="B17" s="270" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="276" t="s">
+      <c r="A18" s="269" t="s">
         <v>449</v>
       </c>
-      <c r="B18" s="277" t="s">
+      <c r="B18" s="270" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="276" t="s">
+      <c r="A19" s="269" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="277" t="s">
+      <c r="B19" s="270" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="276" t="s">
+      <c r="A20" s="269" t="s">
         <v>475</v>
       </c>
-      <c r="B20" s="277" t="s">
+      <c r="B20" s="270" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="276" t="s">
+      <c r="A21" s="269" t="s">
         <v>477</v>
       </c>
-      <c r="B21" s="277" t="s">
+      <c r="B21" s="270" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="276" t="s">
+      <c r="A22" s="269" t="s">
         <v>479</v>
       </c>
-      <c r="B22" s="277" t="s">
+      <c r="B22" s="270" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="276" t="s">
+      <c r="A23" s="269" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="277" t="s">
+      <c r="B23" s="270" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="276" t="s">
+      <c r="A24" s="269" t="s">
         <v>482</v>
       </c>
-      <c r="B24" s="277" t="s">
+      <c r="B24" s="270" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="276" t="s">
+      <c r="A25" s="269" t="s">
         <v>484</v>
       </c>
-      <c r="B25" s="277" t="s">
+      <c r="B25" s="270" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="276" t="s">
+      <c r="A26" s="269" t="s">
         <v>486</v>
       </c>
-      <c r="B26" s="277" t="s">
+      <c r="B26" s="270" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="276" t="s">
+      <c r="A27" s="269" t="s">
         <v>488</v>
       </c>
-      <c r="B27" s="277" t="s">
+      <c r="B27" s="270" t="s">
         <v>489</v>
       </c>
     </row>

</xml_diff>